<commit_message>
stuff ive done so far
</commit_message>
<xml_diff>
--- a/OECD_betterLifeIndex_cpyyyy.xlsx
+++ b/OECD_betterLifeIndex_cpyyyy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dayyanmirza/Desktop/CSC3833_Data_Visualistion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BF0095-019A-FD45-A066-617CFB4762D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088251E8-FA7E-954C-A0EE-F702E0D35A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14300" xr2:uid="{D855B94F-A5ED-F14F-B8BC-BA20E5AD226D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Country</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>United States</t>
-  </si>
-  <si>
-    <t>OECD - Total</t>
   </si>
   <si>
     <t>Brazil</t>
@@ -698,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3243CB-97A4-044F-B548-0960722FF072}">
-  <dimension ref="A1:Y44"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="69" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -711,76 +708,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -3609,294 +3606,217 @@
         <v>14.57</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="4">
-        <v>3</v>
-      </c>
-      <c r="C40" s="4">
-        <v>20.5</v>
-      </c>
-      <c r="D40" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="E40" s="4">
-        <v>30490</v>
-      </c>
-      <c r="F40" s="4">
-        <v>323960</v>
-      </c>
-      <c r="G40" s="4">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="H40" s="4">
-        <v>66</v>
-      </c>
-      <c r="I40" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="J40" s="4">
-        <v>49165</v>
-      </c>
-      <c r="K40" s="4">
-        <v>91</v>
-      </c>
-      <c r="L40" s="4">
-        <v>79</v>
-      </c>
-      <c r="M40" s="4">
-        <v>488</v>
-      </c>
-      <c r="N40" s="4">
-        <v>18</v>
-      </c>
-      <c r="O40" s="4">
-        <v>14</v>
-      </c>
-      <c r="P40" s="4">
-        <v>84</v>
-      </c>
-      <c r="Q40" s="4">
-        <v>2.1</v>
-      </c>
-      <c r="R40" s="4">
-        <v>69</v>
-      </c>
-      <c r="S40" s="4">
-        <v>81</v>
-      </c>
-      <c r="T40" s="4">
-        <v>68</v>
-      </c>
-      <c r="U40" s="4">
+      <c r="B40" s="5">
         <v>6.7</v>
       </c>
-      <c r="V40" s="4">
-        <v>74</v>
-      </c>
-      <c r="W40" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="X40" s="4">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="Y40" s="4">
-        <v>15.07</v>
-      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5">
+        <v>57</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5">
+        <v>83</v>
+      </c>
+      <c r="L40" s="5">
+        <v>57</v>
+      </c>
+      <c r="M40" s="5">
+        <v>400</v>
+      </c>
+      <c r="N40" s="5">
+        <v>16</v>
+      </c>
+      <c r="O40" s="5">
+        <v>11.7</v>
+      </c>
+      <c r="P40" s="5">
+        <v>70</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R40" s="5">
+        <v>80</v>
+      </c>
+      <c r="S40" s="5">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5">
+        <v>6.1</v>
+      </c>
+      <c r="V40" s="5">
+        <v>45</v>
+      </c>
+      <c r="W40" s="5">
+        <v>19</v>
+      </c>
+      <c r="X40" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="Y40" s="5"/>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="5">
-        <v>6.7</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5">
-        <v>57</v>
-      </c>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5">
-        <v>83</v>
-      </c>
-      <c r="L41" s="5">
-        <v>57</v>
-      </c>
-      <c r="M41" s="5">
-        <v>400</v>
-      </c>
-      <c r="N41" s="5">
+      <c r="B41" s="4">
+        <v>13.8</v>
+      </c>
+      <c r="C41" s="4">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D41" s="4">
+        <v>1</v>
+      </c>
+      <c r="E41" s="4">
+        <v>19546</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4">
+        <v>70</v>
+      </c>
+      <c r="I41" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4">
+        <v>89</v>
+      </c>
+      <c r="L41" s="4">
+        <v>95</v>
+      </c>
+      <c r="M41" s="4">
+        <v>481</v>
+      </c>
+      <c r="N41" s="4">
         <v>16</v>
       </c>
-      <c r="O41" s="5">
-        <v>11.7</v>
-      </c>
-      <c r="P41" s="5">
-        <v>70</v>
-      </c>
-      <c r="Q41" s="5">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="R41" s="5">
-        <v>80</v>
-      </c>
-      <c r="S41" s="5">
-        <v>75.900000000000006</v>
-      </c>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5">
-        <v>6.1</v>
-      </c>
-      <c r="V41" s="5">
-        <v>45</v>
-      </c>
-      <c r="W41" s="5">
-        <v>19</v>
-      </c>
-      <c r="X41" s="5">
-        <v>5.6</v>
-      </c>
-      <c r="Y41" s="5"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="O41" s="4">
+        <v>11.8</v>
+      </c>
+      <c r="P41" s="4">
+        <v>62</v>
+      </c>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4">
+        <v>68</v>
+      </c>
+      <c r="S41" s="4">
+        <v>73.2</v>
+      </c>
+      <c r="T41" s="4">
+        <v>43</v>
+      </c>
+      <c r="U41" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="V41" s="4">
+        <v>64</v>
+      </c>
+      <c r="W41" s="4">
+        <v>4.8</v>
+      </c>
+      <c r="X41" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="Y41" s="4"/>
+    </row>
+    <row r="42" spans="1:25" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="4">
-        <v>13.8</v>
-      </c>
-      <c r="C42" s="4">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="D42" s="4">
-        <v>1</v>
-      </c>
-      <c r="E42" s="4">
-        <v>19546</v>
-      </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4">
-        <v>70</v>
-      </c>
-      <c r="I42" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4">
+      <c r="B42" s="5">
+        <v>35.9</v>
+      </c>
+      <c r="C42" s="5">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5">
+        <v>9338</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5">
+        <v>39</v>
+      </c>
+      <c r="I42" s="5">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5">
         <v>89</v>
       </c>
-      <c r="L42" s="4">
-        <v>95</v>
-      </c>
-      <c r="M42" s="4">
-        <v>481</v>
-      </c>
-      <c r="N42" s="4">
-        <v>16</v>
-      </c>
-      <c r="O42" s="4">
-        <v>11.8</v>
-      </c>
-      <c r="P42" s="4">
-        <v>62</v>
-      </c>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4">
-        <v>68</v>
-      </c>
-      <c r="S42" s="4">
-        <v>73.2</v>
-      </c>
-      <c r="T42" s="4">
-        <v>43</v>
-      </c>
-      <c r="U42" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="V42" s="4">
-        <v>64</v>
-      </c>
-      <c r="W42" s="4">
-        <v>4.8</v>
-      </c>
-      <c r="X42" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="Y42" s="4"/>
-    </row>
-    <row r="43" spans="1:25" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5">
-        <v>35.9</v>
-      </c>
-      <c r="C43" s="5">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5">
-        <v>9338</v>
-      </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5">
-        <v>39</v>
-      </c>
-      <c r="I43" s="5">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5">
-        <v>89</v>
-      </c>
-      <c r="L43" s="5">
+      <c r="L42" s="5">
         <v>48</v>
       </c>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5">
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5">
         <v>28.5</v>
       </c>
-      <c r="P43" s="5">
+      <c r="P42" s="5">
         <v>72</v>
       </c>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5">
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5">
         <v>66</v>
       </c>
-      <c r="S43" s="5">
+      <c r="S42" s="5">
         <v>64.2</v>
       </c>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5">
+      <c r="T42" s="5"/>
+      <c r="U42" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="V43" s="5">
+      <c r="V42" s="5">
         <v>40</v>
       </c>
-      <c r="W43" s="5">
+      <c r="W42" s="5">
         <v>13.7</v>
       </c>
-      <c r="X43" s="5">
+      <c r="X42" s="5">
         <v>15.4</v>
       </c>
-      <c r="Y43" s="5"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-      <c r="V44" s="9"/>
-      <c r="W44" s="9"/>
-      <c r="X44" s="9"/>
-      <c r="Y44" s="9"/>
+      <c r="Y42" s="5"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A43" s="8"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>